<commit_message>
Formula Practice Day 2
</commit_message>
<xml_diff>
--- a/04. Formula Practice.xlsx
+++ b/04. Formula Practice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intag\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Excel Practice\Excel-Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFA5BAC-C188-4146-81C4-5C29D7B4ABC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E656A7-0D30-402E-AFD7-565B4AE284A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
   </bookViews>
@@ -2861,8 +2861,8 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="199" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2931,6 +2931,10 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
+      <c r="J2" t="str">
+        <f>TEXT(H2,"mm/dd/yyyy")</f>
+        <v>11/02/2001</v>
+      </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2961,6 +2965,10 @@
       <c r="I3" s="1">
         <v>42287</v>
       </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">TEXT(H3,"mm/dd/yyyy")</f>
+        <v>10/03/1999</v>
+      </c>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2991,6 +2999,10 @@
       <c r="I4" s="1">
         <v>42986</v>
       </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>07/04/2000</v>
+      </c>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3021,6 +3033,10 @@
       <c r="I5" s="1">
         <v>42341</v>
       </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>01/05/2000</v>
+      </c>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3051,6 +3067,10 @@
       <c r="I6" s="1">
         <v>42977</v>
       </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>05/06/2001</v>
+      </c>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3081,6 +3101,10 @@
       <c r="I7" s="1">
         <v>41528</v>
       </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>12/07/1995</v>
+      </c>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3111,6 +3135,10 @@
       <c r="I8" s="1">
         <v>41551</v>
       </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>11/08/2003</v>
+      </c>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3141,6 +3169,10 @@
       <c r="I9" s="1">
         <v>42116</v>
       </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>06/09/2002</v>
+      </c>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3170,6 +3202,10 @@
       </c>
       <c r="I10" s="1">
         <v>40800</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>08/10/2003</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -3191,8 +3227,8 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="157" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3264,6 +3300,10 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
+      <c r="J2" t="str">
+        <f>TRIM(C2)</f>
+        <v>Halpert</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -3293,6 +3333,10 @@
       <c r="I3" s="1">
         <v>42287</v>
       </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">TRIM(C3)</f>
+        <v>Beasley</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -3322,6 +3366,10 @@
       <c r="I4" s="1">
         <v>42986</v>
       </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Schrute</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -3351,6 +3399,10 @@
       <c r="I5" s="1">
         <v>42341</v>
       </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Martin</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -3380,6 +3432,10 @@
       <c r="I6" s="1">
         <v>42977</v>
       </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Flenderson</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -3409,6 +3465,10 @@
       <c r="I7" s="1">
         <v>41528</v>
       </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Scott</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -3438,6 +3498,10 @@
       <c r="I8" s="1">
         <v>41551</v>
       </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Palmer</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -3467,6 +3531,10 @@
       <c r="I9" s="1">
         <v>42116</v>
       </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Hudson</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -3495,6 +3563,10 @@
       </c>
       <c r="I10" s="1">
         <v>40800</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Malone</v>
       </c>
     </row>
   </sheetData>
@@ -3509,8 +3581,8 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView zoomScale="128" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3585,6 +3657,18 @@
       <c r="I2" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="J2" t="str">
+        <f>SUBSTITUTE(I2,"/", "-",1)</f>
+        <v>9-6/2015</v>
+      </c>
+      <c r="K2" t="str">
+        <f>SUBSTITUTE(I2,"/","-",2)</f>
+        <v>9/6-2015</v>
+      </c>
+      <c r="L2" t="str">
+        <f>SUBSTITUTE(I2,"/","-")</f>
+        <v>9-6-2015</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -3614,6 +3698,18 @@
       <c r="I3" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">SUBSTITUTE(I3,"/", "-",1)</f>
+        <v>10-10/2015</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K10" si="1">SUBSTITUTE(I3,"/","-",2)</f>
+        <v>10/10-2015</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L10" si="2">SUBSTITUTE(I3,"/","-")</f>
+        <v>10-10-2015</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -3643,6 +3739,18 @@
       <c r="I4" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>9-8/2017</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>9/8-2017</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v>9-8-2017</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -3672,6 +3780,18 @@
       <c r="I5" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>12-3/2015</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>12/3-2015</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>12-3-2015</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -3701,6 +3821,18 @@
       <c r="I6" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>8-30/2017</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>8/30-2017</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>8-30-2017</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -3730,6 +3862,18 @@
       <c r="I7" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>9-11/2013</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>9/11-2013</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>9-11-2013</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -3759,6 +3903,18 @@
       <c r="I8" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>9-11/2013</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>9/11-2013</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>9-11-2013</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -3788,6 +3944,18 @@
       <c r="I9" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>4-22/2015</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>4/22-2015</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>4-22-2015</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -3816,6 +3984,18 @@
       </c>
       <c r="I10" s="2" t="s">
         <v>62</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>4-22/2015</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>4/22-2015</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>4-22-2015</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>